<commit_message>
Fix Chart.js rendering and forecast table styling for compact, modern UI
</commit_message>
<xml_diff>
--- a/xgb_test_vs_prediction_results.xlsx
+++ b/xgb_test_vs_prediction_results.xlsx
@@ -462,7 +462,7 @@
         <v>4.668443393714001</v>
       </c>
       <c r="C2" t="n">
-        <v>5.268950939178467</v>
+        <v>5.641274452209473</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>4.80551908429409</v>
       </c>
       <c r="C3" t="n">
-        <v>5.109382152557373</v>
+        <v>4.998333930969238</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +484,7 @@
         <v>4.998026813941</v>
       </c>
       <c r="C4" t="n">
-        <v>5.096033573150635</v>
+        <v>5.025818347930908</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +495,7 @@
         <v>5.023363338918999</v>
       </c>
       <c r="C5" t="n">
-        <v>5.078582286834717</v>
+        <v>4.861635208129883</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +506,7 @@
         <v>4.822616096114</v>
       </c>
       <c r="C6" t="n">
-        <v>5.236500263214111</v>
+        <v>4.821127891540527</v>
       </c>
     </row>
     <row r="7">
@@ -517,7 +517,7 @@
         <v>4.429607166733</v>
       </c>
       <c r="C7" t="n">
-        <v>5.326087474822998</v>
+        <v>5.402042865753174</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +528,7 @@
         <v>5.438515029533001</v>
       </c>
       <c r="C8" t="n">
-        <v>5.318022727966309</v>
+        <v>5.098884105682373</v>
       </c>
     </row>
     <row r="9">
@@ -539,7 +539,7 @@
         <v>5.185118522125</v>
       </c>
       <c r="C9" t="n">
-        <v>5.345104694366455</v>
+        <v>5.123974800109863</v>
       </c>
     </row>
     <row r="10">
@@ -550,7 +550,7 @@
         <v>5.692019099825</v>
       </c>
       <c r="C10" t="n">
-        <v>5.493895053863525</v>
+        <v>5.273571014404297</v>
       </c>
     </row>
     <row r="11">
@@ -561,7 +561,7 @@
         <v>5.223532946875</v>
       </c>
       <c r="C11" t="n">
-        <v>5.089605808258057</v>
+        <v>4.882172584533691</v>
       </c>
     </row>
     <row r="12">
@@ -572,7 +572,7 @@
         <v>5.418027537625001</v>
       </c>
       <c r="C12" t="n">
-        <v>5.461669921875</v>
+        <v>5.235822677612305</v>
       </c>
     </row>
     <row r="13">
@@ -583,7 +583,7 @@
         <v>5.840909350502</v>
       </c>
       <c r="C13" t="n">
-        <v>5.184865474700928</v>
+        <v>4.880583763122559</v>
       </c>
     </row>
     <row r="14">
@@ -594,7 +594,7 @@
         <v>5.560000497824999</v>
       </c>
       <c r="C14" t="n">
-        <v>5.043099880218506</v>
+        <v>5.027856349945068</v>
       </c>
     </row>
     <row r="15">
@@ -605,7 +605,7 @@
         <v>5.76415121375</v>
       </c>
       <c r="C15" t="n">
-        <v>5.380143642425537</v>
+        <v>5.113373756408691</v>
       </c>
     </row>
     <row r="16">
@@ -616,7 +616,7 @@
         <v>5.407662430525001</v>
       </c>
       <c r="C16" t="n">
-        <v>5.416504383087158</v>
+        <v>4.987620830535889</v>
       </c>
     </row>
     <row r="17">
@@ -627,7 +627,7 @@
         <v>5.635396825932</v>
       </c>
       <c r="C17" t="n">
-        <v>5.406580448150635</v>
+        <v>4.873868942260742</v>
       </c>
     </row>
     <row r="18">
@@ -638,7 +638,7 @@
         <v>5.904906289082</v>
       </c>
       <c r="C18" t="n">
-        <v>5.072288513183594</v>
+        <v>4.888505935668945</v>
       </c>
     </row>
     <row r="19">
@@ -649,7 +649,7 @@
         <v>5.754983475486</v>
       </c>
       <c r="C19" t="n">
-        <v>5.378955364227295</v>
+        <v>5.317544937133789</v>
       </c>
     </row>
     <row r="20">
@@ -660,7 +660,7 @@
         <v>6.125426000894999</v>
       </c>
       <c r="C20" t="n">
-        <v>5.422359943389893</v>
+        <v>5.417792320251465</v>
       </c>
     </row>
     <row r="21">
@@ -671,7 +671,7 @@
         <v>5.406917101506</v>
       </c>
       <c r="C21" t="n">
-        <v>5.602707386016846</v>
+        <v>5.412067890167236</v>
       </c>
     </row>
     <row r="22">
@@ -682,7 +682,7 @@
         <v>6.574890841338999</v>
       </c>
       <c r="C22" t="n">
-        <v>5.515735626220703</v>
+        <v>5.127096652984619</v>
       </c>
     </row>
     <row r="23">
@@ -693,7 +693,7 @@
         <v>6.405723786886</v>
       </c>
       <c r="C23" t="n">
-        <v>5.110430717468262</v>
+        <v>5.026010036468506</v>
       </c>
     </row>
     <row r="24">
@@ -704,7 +704,7 @@
         <v>6.718604456511001</v>
       </c>
       <c r="C24" t="n">
-        <v>5.440365791320801</v>
+        <v>5.118307590484619</v>
       </c>
     </row>
     <row r="25">
@@ -715,7 +715,7 @@
         <v>6.05485169882</v>
       </c>
       <c r="C25" t="n">
-        <v>5.502627372741699</v>
+        <v>5.123221397399902</v>
       </c>
     </row>
     <row r="26">
@@ -726,7 +726,7 @@
         <v>5.72217794552</v>
       </c>
       <c r="C26" t="n">
-        <v>5.502748012542725</v>
+        <v>5.109638214111328</v>
       </c>
     </row>
     <row r="27">
@@ -737,7 +737,7 @@
         <v>6.699475908175</v>
       </c>
       <c r="C27" t="n">
-        <v>5.493926048278809</v>
+        <v>5.11062479019165</v>
       </c>
     </row>
     <row r="28">
@@ -748,7 +748,7 @@
         <v>5.647809795596</v>
       </c>
       <c r="C28" t="n">
-        <v>5.407448768615723</v>
+        <v>4.963100433349609</v>
       </c>
     </row>
     <row r="29">
@@ -759,7 +759,7 @@
         <v>5.854452414233</v>
       </c>
       <c r="C29" t="n">
-        <v>5.407989025115967</v>
+        <v>4.860276222229004</v>
       </c>
     </row>
     <row r="30">
@@ -770,7 +770,7 @@
         <v>5.460436904519</v>
       </c>
       <c r="C30" t="n">
-        <v>5.404017448425293</v>
+        <v>4.963100433349609</v>
       </c>
     </row>
     <row r="31">
@@ -781,7 +781,7 @@
         <v>5.755830683622917</v>
       </c>
       <c r="C31" t="n">
-        <v>5.613088130950928</v>
+        <v>5.493256092071533</v>
       </c>
     </row>
     <row r="32">
@@ -792,7 +792,7 @@
         <v>5.991571160172917</v>
       </c>
       <c r="C32" t="n">
-        <v>5.442866802215576</v>
+        <v>5.30925464630127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>